<commit_message>
edit outcome name (#13)
</commit_message>
<xml_diff>
--- a/data/nl/outcome_table.xlsx
+++ b/data/nl/outcome_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidpietersz/Documents/GitHub/kansenkloof_NL/data/nl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilsonea/Documents/GitHub/Kansenkloof_Nederland/data/nl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4E44E03-E95D-CA4D-8E80-62C16FB76CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201D8419-5FC6-0349-8954-BF86E5A9D762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="28800" windowHeight="18000" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
   <sheets>
     <sheet name="outcome" sheetId="6" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1695,9 +1693,6 @@
     <t>Klas eindtoets lezen streefniveau</t>
   </si>
   <si>
-    <t>Klas eindteots rekenen streefniveau</t>
-  </si>
-  <si>
     <t>Klas eindtoets taalverzorging streefniveau</t>
   </si>
   <si>
@@ -1708,6 +1703,9 @@
   </si>
   <si>
     <t>c11_class_language</t>
+  </si>
+  <si>
+    <t>Klas eindtoets rekenen streefniveau</t>
   </si>
 </sst>
 </file>
@@ -1865,9 +1863,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1905,7 +1903,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2011,7 +2009,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2153,7 +2151,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2163,7 +2161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F4A81B-7759-BE45-BE6A-975E9F190FD6}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="207" zoomScaleNormal="92" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="92" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -2732,7 +2730,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>540</v>
@@ -2825,7 +2823,7 @@
         <v>538</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>52</v>
@@ -2840,10 +2838,10 @@
         <v>6</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>52</v>
@@ -2861,7 +2859,7 @@
         <v>539</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
new outcomes and area changes
add c16_secondary_class outcomes
assign weesp wijken to amsterdam municipality
</commit_message>
<xml_diff>
--- a/data/nl/outcome_table.xlsx
+++ b/data/nl/outcome_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilsonea/Documents/GitHub/Kansenkloof_Nederland/data/nl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85205157-2A4C-5A4A-8650-BF976DA3B765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D4FE79-F79C-8245-8CAD-AE655F99CE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="22840" windowHeight="19620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21938" uniqueCount="7931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21941" uniqueCount="7933">
   <si>
     <t>prefix_postfix</t>
   </si>
@@ -23650,9 +23650,6 @@
     <t>Schagen (woonkern-Oost en Buitengebied)</t>
   </si>
   <si>
-    <t>Weesp</t>
-  </si>
-  <si>
     <t>045700</t>
   </si>
   <si>
@@ -23840,13 +23837,22 @@
   </si>
   <si>
     <t>174201</t>
+  </si>
+  <si>
+    <t>c16_secondary_class_foreign_born_parents</t>
+  </si>
+  <si>
+    <t>c16_secondary_class_income_above_75th</t>
+  </si>
+  <si>
+    <t>c16_secondary_class_income_below_25th</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -23858,22 +23864,26 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -23884,6 +23894,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -23945,7 +23962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -23968,6 +23985,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23986,9 +24004,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -24026,7 +24044,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -24132,7 +24150,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -24274,7 +24292,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -24282,10 +24300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView topLeftCell="D39" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A22" zoomScale="75" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25793,6 +25811,33 @@
         <v>2</v>
       </c>
     </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B66" s="14" t="s">
+        <v>7930</v>
+      </c>
+      <c r="G66" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B67" s="14" t="s">
+        <v>7931</v>
+      </c>
+      <c r="G67" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B68" s="14" t="s">
+        <v>7932</v>
+      </c>
+      <c r="G68" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B69" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -25803,8 +25848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E4538"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2591" workbookViewId="0">
-      <selection activeCell="E2602" sqref="E2602"/>
+    <sheetView tabSelected="1" topLeftCell="A2075" workbookViewId="0">
+      <selection activeCell="C2117" sqref="C2117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -63631,7 +63676,7 @@
     </row>
     <row r="2423" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2423" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2423" t="s">
         <v>228</v>
@@ -63640,12 +63685,12 @@
         <v>281</v>
       </c>
       <c r="E2423" t="s">
-        <v>7868</v>
+        <v>7867</v>
       </c>
     </row>
     <row r="2424" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2424" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2424" t="s">
         <v>228</v>
@@ -63654,12 +63699,12 @@
         <v>444</v>
       </c>
       <c r="E2424" t="s">
-        <v>7869</v>
+        <v>7868</v>
       </c>
     </row>
     <row r="2425" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2425" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2425" t="s">
         <v>228</v>
@@ -63668,68 +63713,68 @@
         <v>295</v>
       </c>
       <c r="E2425" t="s">
-        <v>7870</v>
+        <v>7869</v>
       </c>
     </row>
     <row r="2426" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2426" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2426" t="s">
         <v>228</v>
       </c>
       <c r="C2426" t="s">
+        <v>7870</v>
+      </c>
+      <c r="E2426" t="s">
         <v>7871</v>
-      </c>
-      <c r="E2426" t="s">
-        <v>7872</v>
       </c>
     </row>
     <row r="2427" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2427" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2427" t="s">
         <v>228</v>
       </c>
       <c r="C2427" t="s">
+        <v>7872</v>
+      </c>
+      <c r="E2427" t="s">
         <v>7873</v>
-      </c>
-      <c r="E2427" t="s">
-        <v>7874</v>
       </c>
     </row>
     <row r="2428" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2428" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2428" t="s">
         <v>228</v>
       </c>
       <c r="C2428" t="s">
+        <v>7874</v>
+      </c>
+      <c r="E2428" t="s">
         <v>7875</v>
-      </c>
-      <c r="E2428" t="s">
-        <v>7876</v>
       </c>
     </row>
     <row r="2429" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2429" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2429" t="s">
         <v>228</v>
       </c>
       <c r="C2429" t="s">
+        <v>7876</v>
+      </c>
+      <c r="E2429" t="s">
         <v>7877</v>
-      </c>
-      <c r="E2429" t="s">
-        <v>7878</v>
       </c>
     </row>
     <row r="2430" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2430" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2430" t="s">
         <v>228</v>
@@ -63738,7 +63783,7 @@
         <v>841</v>
       </c>
       <c r="E2430" t="s">
-        <v>7879</v>
+        <v>7878</v>
       </c>
     </row>
     <row r="2431" spans="1:5" x14ac:dyDescent="0.2">
@@ -65035,58 +65080,58 @@
     </row>
     <row r="2507" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2507" t="s">
+        <v>7879</v>
+      </c>
+      <c r="B2507" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2507" t="s">
         <v>7880</v>
       </c>
-      <c r="B2507" t="s">
-        <v>228</v>
-      </c>
-      <c r="C2507" t="s">
+      <c r="E2507" t="s">
         <v>7881</v>
-      </c>
-      <c r="E2507" t="s">
-        <v>7882</v>
       </c>
     </row>
     <row r="2508" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2508" t="s">
-        <v>7880</v>
+        <v>7879</v>
       </c>
       <c r="B2508" t="s">
         <v>228</v>
       </c>
       <c r="C2508" t="s">
+        <v>7882</v>
+      </c>
+      <c r="E2508" t="s">
         <v>7883</v>
-      </c>
-      <c r="E2508" t="s">
-        <v>7884</v>
       </c>
     </row>
     <row r="2509" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2509" t="s">
-        <v>7880</v>
+        <v>7879</v>
       </c>
       <c r="B2509" t="s">
         <v>228</v>
       </c>
       <c r="C2509" t="s">
+        <v>7884</v>
+      </c>
+      <c r="E2509" t="s">
         <v>7885</v>
-      </c>
-      <c r="E2509" t="s">
-        <v>7886</v>
       </c>
     </row>
     <row r="2510" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2510" t="s">
-        <v>7880</v>
+        <v>7879</v>
       </c>
       <c r="B2510" t="s">
         <v>228</v>
       </c>
       <c r="C2510" t="s">
+        <v>7886</v>
+      </c>
+      <c r="E2510" t="s">
         <v>7887</v>
-      </c>
-      <c r="E2510" t="s">
-        <v>7888</v>
       </c>
     </row>
     <row r="2511" spans="1:5" x14ac:dyDescent="0.2">
@@ -67018,10 +67063,10 @@
         <v>228</v>
       </c>
       <c r="C2624" t="s">
+        <v>7888</v>
+      </c>
+      <c r="E2624" t="s">
         <v>7889</v>
-      </c>
-      <c r="E2624" t="s">
-        <v>7890</v>
       </c>
     </row>
     <row r="2625" spans="1:5" x14ac:dyDescent="0.2">
@@ -67032,10 +67077,10 @@
         <v>228</v>
       </c>
       <c r="C2625" t="s">
+        <v>7890</v>
+      </c>
+      <c r="E2625" t="s">
         <v>7891</v>
-      </c>
-      <c r="E2625" t="s">
-        <v>7892</v>
       </c>
     </row>
     <row r="2626" spans="1:5" x14ac:dyDescent="0.2">
@@ -67046,10 +67091,10 @@
         <v>228</v>
       </c>
       <c r="C2626" t="s">
+        <v>7892</v>
+      </c>
+      <c r="E2626" t="s">
         <v>7893</v>
-      </c>
-      <c r="E2626" t="s">
-        <v>7894</v>
       </c>
     </row>
     <row r="2627" spans="1:5" x14ac:dyDescent="0.2">
@@ -67060,10 +67105,10 @@
         <v>228</v>
       </c>
       <c r="C2627" t="s">
+        <v>7894</v>
+      </c>
+      <c r="E2627" t="s">
         <v>7895</v>
-      </c>
-      <c r="E2627" t="s">
-        <v>7896</v>
       </c>
     </row>
     <row r="2628" spans="1:5" x14ac:dyDescent="0.2">
@@ -67074,10 +67119,10 @@
         <v>228</v>
       </c>
       <c r="C2628" t="s">
+        <v>7896</v>
+      </c>
+      <c r="E2628" t="s">
         <v>7897</v>
-      </c>
-      <c r="E2628" t="s">
-        <v>7898</v>
       </c>
     </row>
     <row r="2629" spans="1:5" x14ac:dyDescent="0.2">
@@ -67088,10 +67133,10 @@
         <v>228</v>
       </c>
       <c r="C2629" t="s">
+        <v>7898</v>
+      </c>
+      <c r="E2629" t="s">
         <v>7899</v>
-      </c>
-      <c r="E2629" t="s">
-        <v>7900</v>
       </c>
     </row>
     <row r="2630" spans="1:5" x14ac:dyDescent="0.2">
@@ -67102,10 +67147,10 @@
         <v>228</v>
       </c>
       <c r="C2630" t="s">
+        <v>7900</v>
+      </c>
+      <c r="E2630" t="s">
         <v>7901</v>
-      </c>
-      <c r="E2630" t="s">
-        <v>7902</v>
       </c>
     </row>
     <row r="2631" spans="1:5" x14ac:dyDescent="0.2">
@@ -67116,10 +67161,10 @@
         <v>228</v>
       </c>
       <c r="C2631" t="s">
+        <v>7902</v>
+      </c>
+      <c r="E2631" t="s">
         <v>7903</v>
-      </c>
-      <c r="E2631" t="s">
-        <v>7904</v>
       </c>
     </row>
     <row r="2632" spans="1:5" x14ac:dyDescent="0.2">
@@ -67130,10 +67175,10 @@
         <v>228</v>
       </c>
       <c r="C2632" t="s">
+        <v>7904</v>
+      </c>
+      <c r="E2632" t="s">
         <v>7905</v>
-      </c>
-      <c r="E2632" t="s">
-        <v>7906</v>
       </c>
     </row>
     <row r="2633" spans="1:5" x14ac:dyDescent="0.2">
@@ -67147,7 +67192,7 @@
         <v>3284</v>
       </c>
       <c r="E2633" t="s">
-        <v>7907</v>
+        <v>7906</v>
       </c>
     </row>
     <row r="2634" spans="1:5" x14ac:dyDescent="0.2">
@@ -67158,10 +67203,10 @@
         <v>228</v>
       </c>
       <c r="C2634" t="s">
+        <v>7907</v>
+      </c>
+      <c r="E2634" t="s">
         <v>7908</v>
-      </c>
-      <c r="E2634" t="s">
-        <v>7909</v>
       </c>
     </row>
     <row r="2635" spans="1:5" x14ac:dyDescent="0.2">
@@ -69212,7 +69257,7 @@
         <v>228</v>
       </c>
       <c r="C2755" t="s">
-        <v>7910</v>
+        <v>7909</v>
       </c>
       <c r="D2755" t="s">
         <v>216</v>
@@ -69263,7 +69308,7 @@
         <v>228</v>
       </c>
       <c r="C2758" t="s">
-        <v>7911</v>
+        <v>7910</v>
       </c>
       <c r="D2758" t="s">
         <v>216</v>
@@ -69297,7 +69342,7 @@
         <v>228</v>
       </c>
       <c r="C2760" t="s">
-        <v>7912</v>
+        <v>7911</v>
       </c>
       <c r="D2760" t="s">
         <v>216</v>
@@ -69314,7 +69359,7 @@
         <v>228</v>
       </c>
       <c r="C2761" t="s">
-        <v>7913</v>
+        <v>7912</v>
       </c>
       <c r="D2761" t="s">
         <v>216</v>
@@ -69331,7 +69376,7 @@
         <v>228</v>
       </c>
       <c r="C2762" t="s">
-        <v>7914</v>
+        <v>7913</v>
       </c>
       <c r="D2762" t="s">
         <v>216</v>
@@ -69535,10 +69580,10 @@
         <v>228</v>
       </c>
       <c r="C2774" t="s">
+        <v>7914</v>
+      </c>
+      <c r="E2774" t="s">
         <v>7915</v>
-      </c>
-      <c r="E2774" t="s">
-        <v>7916</v>
       </c>
     </row>
     <row r="2775" spans="1:5" x14ac:dyDescent="0.2">
@@ -69549,10 +69594,10 @@
         <v>228</v>
       </c>
       <c r="C2775" t="s">
+        <v>7916</v>
+      </c>
+      <c r="E2775" t="s">
         <v>7917</v>
-      </c>
-      <c r="E2775" t="s">
-        <v>7918</v>
       </c>
     </row>
     <row r="2776" spans="1:5" x14ac:dyDescent="0.2">
@@ -78454,7 +78499,7 @@
         <v>228</v>
       </c>
       <c r="C3299" t="s">
-        <v>7919</v>
+        <v>7918</v>
       </c>
       <c r="D3299" t="s">
         <v>275</v>
@@ -78471,7 +78516,7 @@
         <v>228</v>
       </c>
       <c r="C3300" t="s">
-        <v>7920</v>
+        <v>7919</v>
       </c>
       <c r="D3300" t="s">
         <v>275</v>
@@ -78488,7 +78533,7 @@
         <v>228</v>
       </c>
       <c r="C3301" t="s">
-        <v>7921</v>
+        <v>7920</v>
       </c>
       <c r="D3301" t="s">
         <v>275</v>
@@ -83129,7 +83174,7 @@
         <v>228</v>
       </c>
       <c r="C3574" t="s">
-        <v>7922</v>
+        <v>7921</v>
       </c>
       <c r="D3574" t="s">
         <v>275</v>
@@ -83146,7 +83191,7 @@
         <v>228</v>
       </c>
       <c r="C3575" t="s">
-        <v>7923</v>
+        <v>7922</v>
       </c>
       <c r="D3575" t="s">
         <v>275</v>
@@ -83163,7 +83208,7 @@
         <v>228</v>
       </c>
       <c r="C3576" t="s">
-        <v>7924</v>
+        <v>7923</v>
       </c>
       <c r="D3576" t="s">
         <v>275</v>
@@ -83180,7 +83225,7 @@
         <v>228</v>
       </c>
       <c r="C3577" t="s">
-        <v>7925</v>
+        <v>7924</v>
       </c>
       <c r="D3577" t="s">
         <v>275</v>
@@ -83197,7 +83242,7 @@
         <v>228</v>
       </c>
       <c r="C3578" t="s">
-        <v>7926</v>
+        <v>7925</v>
       </c>
       <c r="D3578" t="s">
         <v>275</v>
@@ -83214,7 +83259,7 @@
         <v>228</v>
       </c>
       <c r="C3579" t="s">
-        <v>7927</v>
+        <v>7926</v>
       </c>
       <c r="D3579" t="s">
         <v>275</v>
@@ -83231,7 +83276,7 @@
         <v>228</v>
       </c>
       <c r="C3580" t="s">
-        <v>7928</v>
+        <v>7927</v>
       </c>
       <c r="D3580" t="s">
         <v>275</v>
@@ -89011,13 +89056,13 @@
         <v>228</v>
       </c>
       <c r="C3920" t="s">
-        <v>7929</v>
+        <v>7928</v>
       </c>
       <c r="D3920" t="s">
         <v>447</v>
       </c>
       <c r="E3920" t="s">
-        <v>7930</v>
+        <v>7929</v>
       </c>
     </row>
     <row r="3921" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Download data feature (#39)
* fix the download data button

* new outcomes and area changes

add c16_secondary_class outcomes
assign weesp wijken to amsterdam municipality

* edit child mortality

* edit english data

* edit nl data
</commit_message>
<xml_diff>
--- a/data/nl/outcome_table.xlsx
+++ b/data/nl/outcome_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilsonea/Documents/GitHub/Kansenkloof_Nederland/data/nl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85205157-2A4C-5A4A-8650-BF976DA3B765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D4FE79-F79C-8245-8CAD-AE655F99CE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="22840" windowHeight="19620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21938" uniqueCount="7931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21941" uniqueCount="7933">
   <si>
     <t>prefix_postfix</t>
   </si>
@@ -23650,9 +23650,6 @@
     <t>Schagen (woonkern-Oost en Buitengebied)</t>
   </si>
   <si>
-    <t>Weesp</t>
-  </si>
-  <si>
     <t>045700</t>
   </si>
   <si>
@@ -23840,13 +23837,22 @@
   </si>
   <si>
     <t>174201</t>
+  </si>
+  <si>
+    <t>c16_secondary_class_foreign_born_parents</t>
+  </si>
+  <si>
+    <t>c16_secondary_class_income_above_75th</t>
+  </si>
+  <si>
+    <t>c16_secondary_class_income_below_25th</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -23858,22 +23864,26 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -23884,6 +23894,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -23945,7 +23962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -23968,6 +23985,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23986,9 +24004,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -24026,7 +24044,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -24132,7 +24150,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -24274,7 +24292,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -24282,10 +24300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView topLeftCell="D39" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A22" zoomScale="75" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25793,6 +25811,33 @@
         <v>2</v>
       </c>
     </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B66" s="14" t="s">
+        <v>7930</v>
+      </c>
+      <c r="G66" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B67" s="14" t="s">
+        <v>7931</v>
+      </c>
+      <c r="G67" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B68" s="14" t="s">
+        <v>7932</v>
+      </c>
+      <c r="G68" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B69" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -25803,8 +25848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E4538"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2591" workbookViewId="0">
-      <selection activeCell="E2602" sqref="E2602"/>
+    <sheetView tabSelected="1" topLeftCell="A2075" workbookViewId="0">
+      <selection activeCell="C2117" sqref="C2117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -63631,7 +63676,7 @@
     </row>
     <row r="2423" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2423" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2423" t="s">
         <v>228</v>
@@ -63640,12 +63685,12 @@
         <v>281</v>
       </c>
       <c r="E2423" t="s">
-        <v>7868</v>
+        <v>7867</v>
       </c>
     </row>
     <row r="2424" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2424" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2424" t="s">
         <v>228</v>
@@ -63654,12 +63699,12 @@
         <v>444</v>
       </c>
       <c r="E2424" t="s">
-        <v>7869</v>
+        <v>7868</v>
       </c>
     </row>
     <row r="2425" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2425" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2425" t="s">
         <v>228</v>
@@ -63668,68 +63713,68 @@
         <v>295</v>
       </c>
       <c r="E2425" t="s">
-        <v>7870</v>
+        <v>7869</v>
       </c>
     </row>
     <row r="2426" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2426" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2426" t="s">
         <v>228</v>
       </c>
       <c r="C2426" t="s">
+        <v>7870</v>
+      </c>
+      <c r="E2426" t="s">
         <v>7871</v>
-      </c>
-      <c r="E2426" t="s">
-        <v>7872</v>
       </c>
     </row>
     <row r="2427" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2427" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2427" t="s">
         <v>228</v>
       </c>
       <c r="C2427" t="s">
+        <v>7872</v>
+      </c>
+      <c r="E2427" t="s">
         <v>7873</v>
-      </c>
-      <c r="E2427" t="s">
-        <v>7874</v>
       </c>
     </row>
     <row r="2428" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2428" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2428" t="s">
         <v>228</v>
       </c>
       <c r="C2428" t="s">
+        <v>7874</v>
+      </c>
+      <c r="E2428" t="s">
         <v>7875</v>
-      </c>
-      <c r="E2428" t="s">
-        <v>7876</v>
       </c>
     </row>
     <row r="2429" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2429" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2429" t="s">
         <v>228</v>
       </c>
       <c r="C2429" t="s">
+        <v>7876</v>
+      </c>
+      <c r="E2429" t="s">
         <v>7877</v>
-      </c>
-      <c r="E2429" t="s">
-        <v>7878</v>
       </c>
     </row>
     <row r="2430" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2430" t="s">
-        <v>7867</v>
+        <v>826</v>
       </c>
       <c r="B2430" t="s">
         <v>228</v>
@@ -63738,7 +63783,7 @@
         <v>841</v>
       </c>
       <c r="E2430" t="s">
-        <v>7879</v>
+        <v>7878</v>
       </c>
     </row>
     <row r="2431" spans="1:5" x14ac:dyDescent="0.2">
@@ -65035,58 +65080,58 @@
     </row>
     <row r="2507" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2507" t="s">
+        <v>7879</v>
+      </c>
+      <c r="B2507" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2507" t="s">
         <v>7880</v>
       </c>
-      <c r="B2507" t="s">
-        <v>228</v>
-      </c>
-      <c r="C2507" t="s">
+      <c r="E2507" t="s">
         <v>7881</v>
-      </c>
-      <c r="E2507" t="s">
-        <v>7882</v>
       </c>
     </row>
     <row r="2508" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2508" t="s">
-        <v>7880</v>
+        <v>7879</v>
       </c>
       <c r="B2508" t="s">
         <v>228</v>
       </c>
       <c r="C2508" t="s">
+        <v>7882</v>
+      </c>
+      <c r="E2508" t="s">
         <v>7883</v>
-      </c>
-      <c r="E2508" t="s">
-        <v>7884</v>
       </c>
     </row>
     <row r="2509" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2509" t="s">
-        <v>7880</v>
+        <v>7879</v>
       </c>
       <c r="B2509" t="s">
         <v>228</v>
       </c>
       <c r="C2509" t="s">
+        <v>7884</v>
+      </c>
+      <c r="E2509" t="s">
         <v>7885</v>
-      </c>
-      <c r="E2509" t="s">
-        <v>7886</v>
       </c>
     </row>
     <row r="2510" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2510" t="s">
-        <v>7880</v>
+        <v>7879</v>
       </c>
       <c r="B2510" t="s">
         <v>228</v>
       </c>
       <c r="C2510" t="s">
+        <v>7886</v>
+      </c>
+      <c r="E2510" t="s">
         <v>7887</v>
-      </c>
-      <c r="E2510" t="s">
-        <v>7888</v>
       </c>
     </row>
     <row r="2511" spans="1:5" x14ac:dyDescent="0.2">
@@ -67018,10 +67063,10 @@
         <v>228</v>
       </c>
       <c r="C2624" t="s">
+        <v>7888</v>
+      </c>
+      <c r="E2624" t="s">
         <v>7889</v>
-      </c>
-      <c r="E2624" t="s">
-        <v>7890</v>
       </c>
     </row>
     <row r="2625" spans="1:5" x14ac:dyDescent="0.2">
@@ -67032,10 +67077,10 @@
         <v>228</v>
       </c>
       <c r="C2625" t="s">
+        <v>7890</v>
+      </c>
+      <c r="E2625" t="s">
         <v>7891</v>
-      </c>
-      <c r="E2625" t="s">
-        <v>7892</v>
       </c>
     </row>
     <row r="2626" spans="1:5" x14ac:dyDescent="0.2">
@@ -67046,10 +67091,10 @@
         <v>228</v>
       </c>
       <c r="C2626" t="s">
+        <v>7892</v>
+      </c>
+      <c r="E2626" t="s">
         <v>7893</v>
-      </c>
-      <c r="E2626" t="s">
-        <v>7894</v>
       </c>
     </row>
     <row r="2627" spans="1:5" x14ac:dyDescent="0.2">
@@ -67060,10 +67105,10 @@
         <v>228</v>
       </c>
       <c r="C2627" t="s">
+        <v>7894</v>
+      </c>
+      <c r="E2627" t="s">
         <v>7895</v>
-      </c>
-      <c r="E2627" t="s">
-        <v>7896</v>
       </c>
     </row>
     <row r="2628" spans="1:5" x14ac:dyDescent="0.2">
@@ -67074,10 +67119,10 @@
         <v>228</v>
       </c>
       <c r="C2628" t="s">
+        <v>7896</v>
+      </c>
+      <c r="E2628" t="s">
         <v>7897</v>
-      </c>
-      <c r="E2628" t="s">
-        <v>7898</v>
       </c>
     </row>
     <row r="2629" spans="1:5" x14ac:dyDescent="0.2">
@@ -67088,10 +67133,10 @@
         <v>228</v>
       </c>
       <c r="C2629" t="s">
+        <v>7898</v>
+      </c>
+      <c r="E2629" t="s">
         <v>7899</v>
-      </c>
-      <c r="E2629" t="s">
-        <v>7900</v>
       </c>
     </row>
     <row r="2630" spans="1:5" x14ac:dyDescent="0.2">
@@ -67102,10 +67147,10 @@
         <v>228</v>
       </c>
       <c r="C2630" t="s">
+        <v>7900</v>
+      </c>
+      <c r="E2630" t="s">
         <v>7901</v>
-      </c>
-      <c r="E2630" t="s">
-        <v>7902</v>
       </c>
     </row>
     <row r="2631" spans="1:5" x14ac:dyDescent="0.2">
@@ -67116,10 +67161,10 @@
         <v>228</v>
       </c>
       <c r="C2631" t="s">
+        <v>7902</v>
+      </c>
+      <c r="E2631" t="s">
         <v>7903</v>
-      </c>
-      <c r="E2631" t="s">
-        <v>7904</v>
       </c>
     </row>
     <row r="2632" spans="1:5" x14ac:dyDescent="0.2">
@@ -67130,10 +67175,10 @@
         <v>228</v>
       </c>
       <c r="C2632" t="s">
+        <v>7904</v>
+      </c>
+      <c r="E2632" t="s">
         <v>7905</v>
-      </c>
-      <c r="E2632" t="s">
-        <v>7906</v>
       </c>
     </row>
     <row r="2633" spans="1:5" x14ac:dyDescent="0.2">
@@ -67147,7 +67192,7 @@
         <v>3284</v>
       </c>
       <c r="E2633" t="s">
-        <v>7907</v>
+        <v>7906</v>
       </c>
     </row>
     <row r="2634" spans="1:5" x14ac:dyDescent="0.2">
@@ -67158,10 +67203,10 @@
         <v>228</v>
       </c>
       <c r="C2634" t="s">
+        <v>7907</v>
+      </c>
+      <c r="E2634" t="s">
         <v>7908</v>
-      </c>
-      <c r="E2634" t="s">
-        <v>7909</v>
       </c>
     </row>
     <row r="2635" spans="1:5" x14ac:dyDescent="0.2">
@@ -69212,7 +69257,7 @@
         <v>228</v>
       </c>
       <c r="C2755" t="s">
-        <v>7910</v>
+        <v>7909</v>
       </c>
       <c r="D2755" t="s">
         <v>216</v>
@@ -69263,7 +69308,7 @@
         <v>228</v>
       </c>
       <c r="C2758" t="s">
-        <v>7911</v>
+        <v>7910</v>
       </c>
       <c r="D2758" t="s">
         <v>216</v>
@@ -69297,7 +69342,7 @@
         <v>228</v>
       </c>
       <c r="C2760" t="s">
-        <v>7912</v>
+        <v>7911</v>
       </c>
       <c r="D2760" t="s">
         <v>216</v>
@@ -69314,7 +69359,7 @@
         <v>228</v>
       </c>
       <c r="C2761" t="s">
-        <v>7913</v>
+        <v>7912</v>
       </c>
       <c r="D2761" t="s">
         <v>216</v>
@@ -69331,7 +69376,7 @@
         <v>228</v>
       </c>
       <c r="C2762" t="s">
-        <v>7914</v>
+        <v>7913</v>
       </c>
       <c r="D2762" t="s">
         <v>216</v>
@@ -69535,10 +69580,10 @@
         <v>228</v>
       </c>
       <c r="C2774" t="s">
+        <v>7914</v>
+      </c>
+      <c r="E2774" t="s">
         <v>7915</v>
-      </c>
-      <c r="E2774" t="s">
-        <v>7916</v>
       </c>
     </row>
     <row r="2775" spans="1:5" x14ac:dyDescent="0.2">
@@ -69549,10 +69594,10 @@
         <v>228</v>
       </c>
       <c r="C2775" t="s">
+        <v>7916</v>
+      </c>
+      <c r="E2775" t="s">
         <v>7917</v>
-      </c>
-      <c r="E2775" t="s">
-        <v>7918</v>
       </c>
     </row>
     <row r="2776" spans="1:5" x14ac:dyDescent="0.2">
@@ -78454,7 +78499,7 @@
         <v>228</v>
       </c>
       <c r="C3299" t="s">
-        <v>7919</v>
+        <v>7918</v>
       </c>
       <c r="D3299" t="s">
         <v>275</v>
@@ -78471,7 +78516,7 @@
         <v>228</v>
       </c>
       <c r="C3300" t="s">
-        <v>7920</v>
+        <v>7919</v>
       </c>
       <c r="D3300" t="s">
         <v>275</v>
@@ -78488,7 +78533,7 @@
         <v>228</v>
       </c>
       <c r="C3301" t="s">
-        <v>7921</v>
+        <v>7920</v>
       </c>
       <c r="D3301" t="s">
         <v>275</v>
@@ -83129,7 +83174,7 @@
         <v>228</v>
       </c>
       <c r="C3574" t="s">
-        <v>7922</v>
+        <v>7921</v>
       </c>
       <c r="D3574" t="s">
         <v>275</v>
@@ -83146,7 +83191,7 @@
         <v>228</v>
       </c>
       <c r="C3575" t="s">
-        <v>7923</v>
+        <v>7922</v>
       </c>
       <c r="D3575" t="s">
         <v>275</v>
@@ -83163,7 +83208,7 @@
         <v>228</v>
       </c>
       <c r="C3576" t="s">
-        <v>7924</v>
+        <v>7923</v>
       </c>
       <c r="D3576" t="s">
         <v>275</v>
@@ -83180,7 +83225,7 @@
         <v>228</v>
       </c>
       <c r="C3577" t="s">
-        <v>7925</v>
+        <v>7924</v>
       </c>
       <c r="D3577" t="s">
         <v>275</v>
@@ -83197,7 +83242,7 @@
         <v>228</v>
       </c>
       <c r="C3578" t="s">
-        <v>7926</v>
+        <v>7925</v>
       </c>
       <c r="D3578" t="s">
         <v>275</v>
@@ -83214,7 +83259,7 @@
         <v>228</v>
       </c>
       <c r="C3579" t="s">
-        <v>7927</v>
+        <v>7926</v>
       </c>
       <c r="D3579" t="s">
         <v>275</v>
@@ -83231,7 +83276,7 @@
         <v>228</v>
       </c>
       <c r="C3580" t="s">
-        <v>7928</v>
+        <v>7927</v>
       </c>
       <c r="D3580" t="s">
         <v>275</v>
@@ -89011,13 +89056,13 @@
         <v>228</v>
       </c>
       <c r="C3920" t="s">
-        <v>7929</v>
+        <v>7928</v>
       </c>
       <c r="D3920" t="s">
         <v>447</v>
       </c>
       <c r="E3920" t="s">
-        <v>7930</v>
+        <v>7929</v>
       </c>
     </row>
     <row r="3921" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>